<commit_message>
add VR Template result figure
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27A887B-A19B-1245-8A5E-A50B8253E133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1961AE-4BB5-624A-82F5-FC6C02E9D9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25420" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="19640" yWindow="6280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-Interactobot" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Time</t>
   </si>
   <si>
     <t>Coverage</t>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Run 3</t>
+  </si>
+  <si>
+    <t>Run 4</t>
+  </si>
+  <si>
+    <t>Run 5</t>
   </si>
 </sst>
 </file>
@@ -523,9 +538,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -884,21 +898,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90EC9EA9-DAEC-BA47-AE45-0297A61EDF45}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -906,7 +920,7 @@
       <c r="A2">
         <v>30</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <f>2/11</f>
         <v>0.18181818181818182</v>
       </c>
@@ -915,7 +929,7 @@
       <c r="A3">
         <v>60</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <f>7/11</f>
         <v>0.63636363636363635</v>
       </c>
@@ -924,7 +938,7 @@
       <c r="A4">
         <v>90</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <f>10/11</f>
         <v>0.90909090909090906</v>
       </c>
@@ -933,7 +947,7 @@
       <c r="A5">
         <v>120</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <f>10/11</f>
         <v>0.90909090909090906</v>
       </c>
@@ -942,7 +956,7 @@
       <c r="A6">
         <v>150</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <f t="shared" ref="B6:B11" si="0">10/11</f>
         <v>0.90909090909090906</v>
       </c>
@@ -951,7 +965,7 @@
       <c r="A7">
         <v>180</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
@@ -960,7 +974,7 @@
       <c r="A8">
         <v>210</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
@@ -969,7 +983,7 @@
       <c r="A9">
         <v>240</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
@@ -978,7 +992,7 @@
       <c r="A10">
         <v>270</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
@@ -987,7 +1001,7 @@
       <c r="A11">
         <v>300</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
@@ -1000,68 +1014,282 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56133-D0E1-9841-A980-CD948866944A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>SUM(C2:G2)/5/11</f>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>60</v>
       </c>
-      <c r="B2" s="1">
-        <f>7/11</f>
-        <v>0.63636363636363635</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B11" si="0">SUM(C3:G3)/5/11</f>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>120</v>
       </c>
-      <c r="B3" s="1">
-        <f>10/11</f>
-        <v>0.90909090909090906</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>180</v>
       </c>
-      <c r="B4" s="1">
-        <f>10/11</f>
-        <v>0.90909090909090906</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14545454545454548</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14545454545454548</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>240</v>
       </c>
-      <c r="B5" s="1">
-        <f>10/11</f>
-        <v>0.90909090909090906</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>300</v>
       </c>
-      <c r="B6" s="1">
-        <f>10/11</f>
-        <v>0.90909090909090906</v>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add evaluation results scene 1, 2, 6
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1961AE-4BB5-624A-82F5-FC6C02E9D9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B5FFA3-03E7-7348-8328-DD4A7A3845E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19640" yWindow="6280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="-26700" yWindow="5840" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-Interactobot" sheetId="1" r:id="rId1"/>
     <sheet name="VR Template-Interactobot_rand" sheetId="2" r:id="rId2"/>
+    <sheet name="XRI Assets-Interactobot" sheetId="3" r:id="rId3"/>
+    <sheet name="XRI Assets-Interactobot_rand" sheetId="4" r:id="rId4"/>
+    <sheet name="EscapeProto-Interactobot" sheetId="5" r:id="rId5"/>
+    <sheet name="EscapeProto-Interactobot_rand" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
   <si>
     <t>Time</t>
   </si>
@@ -899,7 +903,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1016,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56133-D0E1-9841-A980-CD948866944A}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1292,4 +1296,791 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15936B2-1676-F940-AF23-CB2DF196DD0F}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>3/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f>6/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f>11/11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:B11" si="0">11/11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AC60EC-A1F1-6E44-A987-52E44B65BC70}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>SUM(C2:G2)/5/11</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B11" si="0">SUM(C3:G3)/5/11</f>
+        <v>1.8181818181818184E-2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6363636363636369E-2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6363636363636369E-2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6363636363636369E-2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2727272727272738E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECC8B0B-CBDC-5847-BB6E-8516ACDBBA82}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>7/19</f>
+        <v>0.36842105263157893</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f>9/19</f>
+        <v>0.47368421052631576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f>14/19</f>
+        <v>0.73684210526315785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f>16/19</f>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ref="B6:B11" si="0">16/19</f>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD08576-EC75-9547-97E5-385F2DCC0F5B}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>SUM(C2:G2)/5/11</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B11" si="0">SUM(C3:G3)/5/11</f>
+        <v>1.8181818181818184E-2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8181818181818184E-2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6363636363636369E-2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6363636363636369E-2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add RQ3 result scene 5
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B5FFA3-03E7-7348-8328-DD4A7A3845E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA33AA4-2D56-4F41-BD02-1706148FDE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26700" yWindow="5840" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="5180" yWindow="5480" windowWidth="28040" windowHeight="17440" firstSheet="2" activeTab="7" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-Interactobot" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="XRI Assets-Interactobot_rand" sheetId="4" r:id="rId4"/>
     <sheet name="EscapeProto-Interactobot" sheetId="5" r:id="rId5"/>
     <sheet name="EscapeProto-Interactobot_rand" sheetId="6" r:id="rId6"/>
+    <sheet name="GameJam-Interactobot" sheetId="7" r:id="rId7"/>
+    <sheet name="GameJam-Interactobot_rand" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
   <si>
     <t>Time</t>
   </si>
@@ -1697,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECC8B0B-CBDC-5847-BB6E-8516ACDBBA82}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1803,6 +1805,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1811,7 +1814,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G11"/>
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2083,4 +2086,395 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B3A1AD-33CF-4340-A536-B015D8DA4726}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>3/32</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f>6/32</f>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f>11/32</f>
+        <v>0.34375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f>15/32</f>
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f>19/32</f>
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f>23/32</f>
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f>27/32</f>
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f>29/32</f>
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ref="B10:B11" si="0">29/32</f>
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.90625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D0CA9D-08E8-E74D-9EAB-753CF0FAFD9E}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>SUM(C2:G2)/5/11</f>
+        <v>3.6363636363636369E-2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B11" si="0">SUM(C3:G3)/5/11</f>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2727272727272738E-2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10909090909090909</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update results of scene 1
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D1D889-AAE2-D842-BA09-14C5F899E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FF027A-1107-8C4C-B64C-778EC01CF4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="3320" windowWidth="31640" windowHeight="19640" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="4020" yWindow="4320" windowWidth="31640" windowHeight="19640" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-InteractoBot" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="21">
   <si>
     <t>Time</t>
   </si>
@@ -62,12 +62,54 @@
   <si>
     <t>Run 5</t>
   </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Grab</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1/1</t>
+  </si>
+  <si>
+    <t>8/8</t>
+  </si>
+  <si>
+    <t>9/9</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>0/1</t>
+  </si>
+  <si>
+    <t>1/8</t>
+  </si>
+  <si>
+    <t>1/9</t>
+  </si>
+  <si>
+    <t>0/8</t>
+  </si>
+  <si>
+    <t>0/9</t>
+  </si>
+  <si>
+    <t>0.2/8</t>
+  </si>
+  <si>
+    <t>0.2/9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -198,6 +240,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -544,9 +592,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,64 +951,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90EC9EA9-DAEC-BA47-AE45-0297A61EDF45}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="3" max="7" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="14" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
       <c r="B2" s="1">
-        <f>3/9</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <f>AVERAGE(C2:G2)</f>
+        <v>0.53333333333333344</v>
+      </c>
+      <c r="C2" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D2" s="1">
+        <f>6/9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E2" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F2" s="1">
+        <f>5/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G2" s="1">
+        <f>5/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1">
+        <v>58.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
       <c r="B3" s="1">
+        <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
+        <v>0.97777777777777786</v>
+      </c>
+      <c r="C3" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <f>8/9</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F3" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>90</v>
       </c>
       <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <f>9/9</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:E21" si="1">9/9</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:G21" si="2">9/9</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="1">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>120</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ref="B5:B21" si="0">9/9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:C21" si="3">9/9</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>150</v>
       </c>
@@ -967,8 +1185,43 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="1">
+        <v>53.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>180</v>
       </c>
@@ -976,8 +1229,44 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="1">
+        <f>AVERAGE(M2:M6)</f>
+        <v>53.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>210</v>
       </c>
@@ -985,8 +1274,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>240</v>
       </c>
@@ -994,8 +1303,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>270</v>
       </c>
@@ -1003,8 +1332,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>300</v>
       </c>
@@ -1012,8 +1361,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>330</v>
       </c>
@@ -1021,8 +1390,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>360</v>
       </c>
@@ -1030,8 +1419,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>390</v>
       </c>
@@ -1039,8 +1448,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>420</v>
       </c>
@@ -1048,8 +1477,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>450</v>
       </c>
@@ -1057,8 +1506,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>480</v>
       </c>
@@ -1066,8 +1535,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>510</v>
       </c>
@@ -1075,8 +1564,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>540</v>
       </c>
@@ -1084,8 +1593,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>570</v>
       </c>
@@ -1093,8 +1622,28 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>600</v>
       </c>
@@ -1102,8 +1651,29 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="C21" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1111,278 +1681,713 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56133-D0E1-9841-A980-CD948866944A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G11"/>
+    <sheetView zoomScale="159" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="2" max="7" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
       <c r="B2" s="1">
-        <f>SUM(C2:G2)/5/11</f>
-        <v>5.4545454545454543E-2</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+        <f>SUM(C2:G2)/5</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B11" si="0">SUM(C3:G3)/5/11</f>
-        <v>5.4545454545454543E-2</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" ref="B3:B21" si="0">SUM(C3:G3)/5</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:G18" si="1">0/9</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>90</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>120</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>0.10909090909090909</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>150</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>0.10909090909090909</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>180</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0.14545454545454548</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>210</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>0.14545454545454548</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>240</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:C21" si="2">1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>270</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>300</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>330</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>360</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>390</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>420</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>450</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>480</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>510</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>540</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:G21" si="3">0/9</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>570</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>600</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>2.222222222222222E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update results Scene 1
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38389CCD-F2B5-F846-B204-831742B3A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18941B1-4092-AB46-88D3-5E3868684FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" firstSheet="1" activeTab="14" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" activeTab="1" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-InteractoBot" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="54">
   <si>
     <t>Time</t>
   </si>
@@ -93,24 +93,6 @@
   </si>
   <si>
     <t>0/1</t>
-  </si>
-  <si>
-    <t>1/8</t>
-  </si>
-  <si>
-    <t>1/9</t>
-  </si>
-  <si>
-    <t>0/8</t>
-  </si>
-  <si>
-    <t>0/9</t>
-  </si>
-  <si>
-    <t>0.2/8</t>
-  </si>
-  <si>
-    <t>0.2/9</t>
   </si>
   <si>
     <t>2/2</t>
@@ -198,6 +180,36 @@
   </si>
   <si>
     <t xml:space="preserve">Execution Time </t>
+  </si>
+  <si>
+    <t>3/8</t>
+  </si>
+  <si>
+    <t>4/8</t>
+  </si>
+  <si>
+    <t>4/9</t>
+  </si>
+  <si>
+    <t>5/8</t>
+  </si>
+  <si>
+    <t>5/9</t>
+  </si>
+  <si>
+    <t>3/9</t>
+  </si>
+  <si>
+    <t>2/8</t>
+  </si>
+  <si>
+    <t>2/9</t>
+  </si>
+  <si>
+    <t>3.6/8</t>
+  </si>
+  <si>
+    <t>3.6/9</t>
   </si>
 </sst>
 </file>
@@ -2138,13 +2150,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1">
         <v>136.1</v>
@@ -2182,13 +2194,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M3" s="1">
         <v>133.1</v>
@@ -2226,13 +2238,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M4" s="1">
         <v>130.5</v>
@@ -2270,13 +2282,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M5" s="1">
         <v>134.4</v>
@@ -2314,13 +2326,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M6" s="1">
         <v>133.69999999999999</v>
@@ -2358,13 +2370,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(M2:M6)</f>
@@ -2875,10 +2887,10 @@
         <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1">
         <v>233.7</v>
@@ -2919,10 +2931,10 @@
         <v>11</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M3" s="1">
         <v>232</v>
@@ -2963,10 +2975,10 @@
         <v>11</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M4" s="1">
         <v>231.4</v>
@@ -3007,10 +3019,10 @@
         <v>11</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M5" s="1">
         <v>231.4</v>
@@ -3051,10 +3063,10 @@
         <v>11</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M6" s="1">
         <v>236.6</v>
@@ -3095,10 +3107,10 @@
         <v>11</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(M2:M6)</f>
@@ -3533,7 +3545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E49D7EB-C7D2-824A-8D7A-8EA3762D7E06}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3559,7 +3571,7 @@
         <v>0.43009606846725462</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1">
         <f>AVERAGE('VR Template-InteractoBot'!M7, 'XRI Assets-InteractoBot'!M7, 'EscapeProto-InteractoBot'!M7, 'EscapeRoom-InteractoBot'!M7, 'GameJam-InteractoBot'!M7, 'XRI Kit-InteractoBot'!M7, 'XRI Examples-InteractoBot'!M7)</f>
@@ -3758,13 +3770,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56133-D0E1-9841-A980-CD948866944A}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="7" width="10.83203125" style="1"/>
+    <col min="9" max="12" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -3789,13 +3802,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2"/>
@@ -3807,7 +3820,7 @@
       </c>
       <c r="B2" s="1">
         <f>SUM(C2:G2)/5</f>
-        <v>0</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="C2" s="1">
         <f>0/9</f>
@@ -3822,12 +3835,12 @@
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <f>0/9</f>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="G2" s="1">
-        <f>0/9</f>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
@@ -3836,10 +3849,10 @@
         <v>14</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -3850,27 +3863,27 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B21" si="0">SUM(C3:G3)/5</f>
-        <v>0</v>
+        <v>0.11111111111111112</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:G18" si="1">0/9</f>
+        <f>0/9</f>
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" si="1"/>
+        <f>0/9</f>
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" si="1"/>
+        <f>0/9</f>
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>3</v>
@@ -3878,11 +3891,11 @@
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
+      <c r="K3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -3893,27 +3906,27 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.17777777777777776</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="1"/>
+        <f>0/9</f>
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
@@ -3921,11 +3934,11 @@
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
+      <c r="K4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -3936,27 +3949,27 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24444444444444446</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
@@ -3964,11 +3977,11 @@
       <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
+      <c r="K5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -3979,27 +3992,27 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24444444444444446</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="D6:F21" si="1">4/9</f>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
@@ -4007,11 +4020,11 @@
       <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
+      <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -4022,27 +4035,27 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
@@ -4050,11 +4063,11 @@
       <c r="J7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" t="s">
-        <v>20</v>
+      <c r="K7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -4065,27 +4078,27 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="C8" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E8" s="1">
         <f>1/9</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -4094,27 +4107,27 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.31111111111111106</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ref="C9:C21" si="2">1/9</f>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -4123,27 +4136,27 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.31111111111111106</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -4152,27 +4165,27 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -4181,27 +4194,27 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.35555555555555551</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -4210,27 +4223,27 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.35555555555555551</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -4239,27 +4252,27 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.35555555555555551</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -4268,27 +4281,27 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -4297,27 +4310,27 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4326,27 +4339,27 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -4355,27 +4368,27 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4384,27 +4397,27 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" ref="D19:G21" si="3">0/9</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -4413,27 +4426,27 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4442,27 +4455,27 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>2.222222222222222E-2</v>
+        <v>0.4</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1111111111111111</v>
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>5/9</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>
@@ -4551,10 +4564,10 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>11</v>
@@ -4595,10 +4608,10 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>11</v>
@@ -4639,10 +4652,10 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>11</v>
@@ -4683,10 +4696,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>11</v>
@@ -4727,10 +4740,10 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
@@ -4771,10 +4784,10 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>11</v>
@@ -5268,10 +5281,10 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>11</v>
@@ -5307,10 +5320,10 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>11</v>
@@ -5346,10 +5359,10 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>11</v>
@@ -5385,10 +5398,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>11</v>
@@ -5424,10 +5437,10 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>11</v>
@@ -5463,10 +5476,10 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>11</v>
@@ -5705,13 +5718,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1">
         <v>52.4</v>
@@ -5749,13 +5762,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1">
         <v>45.4</v>
@@ -5793,13 +5806,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1">
         <v>48.8</v>
@@ -5837,13 +5850,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M5" s="1">
         <v>50.4</v>
@@ -5881,13 +5894,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M6" s="1">
         <v>49.5</v>
@@ -5925,13 +5938,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(M2:M6)</f>
@@ -6738,7 +6751,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -6773,19 +6786,19 @@
         <v>2</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="M2" s="4">
         <v>533.9</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -6820,19 +6833,19 @@
         <v>3</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="M3" s="4">
         <v>446.4</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -6867,19 +6880,19 @@
         <v>4</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M4" s="4">
         <v>422.8</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -6914,19 +6927,19 @@
         <v>5</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="M5" s="4">
         <v>448.5</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -6961,19 +6974,19 @@
         <v>6</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="M6" s="4">
         <v>447</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -7008,20 +7021,20 @@
         <v>13</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M7" s="4">
         <f>AVERAGE(M2:M6)</f>
         <v>459.71999999999997</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -7343,7 +7356,7 @@
         <v>0.94656488549618323</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" ref="C4:G21" si="2">17/17</f>
+        <f t="shared" ref="F17:F21" si="2">17/17</f>
         <v>1</v>
       </c>
       <c r="G17" s="4">
@@ -7583,13 +7596,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M2" s="1">
         <v>90.6</v>
@@ -7627,13 +7640,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M3" s="1">
         <v>94.6</v>
@@ -7671,13 +7684,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M4" s="1">
         <v>91</v>
@@ -7715,13 +7728,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M5" s="1">
         <v>96.5</v>
@@ -7759,13 +7772,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M6" s="1">
         <v>89.3</v>
@@ -7803,13 +7816,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(M2:M6)</f>

</xml_diff>

<commit_message>
parse duplicated game object names in XUI graph
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18941B1-4092-AB46-88D3-5E3868684FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC9888E-DFF0-C749-94AE-0879CDB1E2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" activeTab="1" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="3" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-InteractoBot" sheetId="1" r:id="rId1"/>
@@ -771,9 +771,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -811,7 +811,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -917,7 +917,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1059,7 +1059,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3770,7 +3770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56133-D0E1-9841-A980-CD948866944A}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -3823,15 +3823,15 @@
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="C2" s="1">
-        <f>0/9</f>
+        <f t="shared" ref="C2:E3" si="0">0/9</f>
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <f>0/9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <f>0/9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F2" s="1">
@@ -3862,27 +3862,27 @@
         <v>60</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B21" si="0">SUM(C3:G3)/5</f>
+        <f t="shared" ref="B3:B21" si="1">SUM(C3:G3)/5</f>
         <v>0.11111111111111112</v>
       </c>
       <c r="C3" s="1">
-        <f>0/9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f>0/9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <f>0/9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f>2/9</f>
+        <f t="shared" ref="F3:F8" si="2">2/9</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="G3" s="1">
-        <f>3/9</f>
+        <f t="shared" ref="G3:G21" si="3">3/9</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -3905,7 +3905,7 @@
         <v>90</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17777777777777776</v>
       </c>
       <c r="C4" s="1">
@@ -3921,11 +3921,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="F4" s="1">
-        <f>2/9</f>
+        <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="G4" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -3948,7 +3948,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24444444444444446</v>
       </c>
       <c r="C5" s="1">
@@ -3964,11 +3964,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="F5" s="1">
-        <f>2/9</f>
+        <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="G5" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -3991,7 +3991,7 @@
         <v>150</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24444444444444446</v>
       </c>
       <c r="C6" s="1">
@@ -3999,7 +3999,7 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:F21" si="1">4/9</f>
+        <f t="shared" ref="D6:F21" si="4">4/9</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="E6" s="1">
@@ -4007,11 +4007,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="F6" s="1">
-        <f>2/9</f>
+        <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="G6" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -4034,15 +4034,15 @@
         <v>180</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="C7" s="1">
-        <f>2/9</f>
+        <f t="shared" ref="C7:C21" si="5">2/9</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E7" s="1">
@@ -4050,11 +4050,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="F7" s="1">
-        <f>2/9</f>
+        <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="G7" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -4077,15 +4077,15 @@
         <v>210</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="C8" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E8" s="1">
@@ -4093,11 +4093,11 @@
         <v>0.1111111111111111</v>
       </c>
       <c r="F8" s="1">
-        <f>2/9</f>
+        <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="G8" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4106,15 +4106,15 @@
         <v>240</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.31111111111111106</v>
       </c>
       <c r="C9" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E9" s="1">
@@ -4122,11 +4122,11 @@
         <v>0.22222222222222221</v>
       </c>
       <c r="F9" s="1">
-        <f>3/9</f>
+        <f t="shared" ref="F9:F14" si="6">3/9</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="G9" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4135,15 +4135,15 @@
         <v>270</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.31111111111111106</v>
       </c>
       <c r="C10" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E10" s="1">
@@ -4151,11 +4151,11 @@
         <v>0.22222222222222221</v>
       </c>
       <c r="F10" s="1">
-        <f>3/9</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G10" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4164,15 +4164,15 @@
         <v>300</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C11" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E11" s="1">
@@ -4180,11 +4180,11 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="F11" s="1">
-        <f>3/9</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G11" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4193,27 +4193,27 @@
         <v>330</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.35555555555555551</v>
       </c>
       <c r="C12" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F12" s="1">
-        <f>3/9</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G12" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4222,27 +4222,27 @@
         <v>360</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.35555555555555551</v>
       </c>
       <c r="C13" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F13" s="1">
-        <f>3/9</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G13" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4251,27 +4251,27 @@
         <v>390</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.35555555555555551</v>
       </c>
       <c r="C14" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F14" s="1">
-        <f>3/9</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="G14" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4280,27 +4280,27 @@
         <v>420</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37777777777777777</v>
       </c>
       <c r="C15" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G15" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4309,27 +4309,27 @@
         <v>450</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37777777777777777</v>
       </c>
       <c r="C16" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G16" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4338,27 +4338,27 @@
         <v>480</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37777777777777777</v>
       </c>
       <c r="C17" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G17" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4367,27 +4367,27 @@
         <v>510</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37777777777777777</v>
       </c>
       <c r="C18" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G18" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4396,27 +4396,27 @@
         <v>540</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37777777777777777</v>
       </c>
       <c r="C19" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G19" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4425,27 +4425,27 @@
         <v>570</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37777777777777777</v>
       </c>
       <c r="C20" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="G20" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -4454,19 +4454,19 @@
         <v>600</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="C21" s="1">
-        <f>2/9</f>
+        <f t="shared" si="5"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F21" s="1">
@@ -4474,7 +4474,7 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="G21" s="1">
-        <f>3/9</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -5213,8 +5213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AC60EC-A1F1-6E44-A987-52E44B65BC70}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
complete results with RQ3
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1BECA8-3381-354B-82A1-3214DAD37DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B2AD0-2F34-5A48-BA90-252B0931E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" firstSheet="8" activeTab="9" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="6140" yWindow="500" windowWidth="28800" windowHeight="26520" firstSheet="8" activeTab="15" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-InteractoBot" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="Average-InteractoBot" sheetId="15" r:id="rId15"/>
     <sheet name="Average-Random" sheetId="16" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,6 +39,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="106">
   <si>
     <t>Time</t>
   </si>
@@ -305,6 +306,66 @@
   </si>
   <si>
     <t>5/24</t>
+  </si>
+  <si>
+    <t>8/21</t>
+  </si>
+  <si>
+    <t>8/24</t>
+  </si>
+  <si>
+    <t>6/21</t>
+  </si>
+  <si>
+    <t>6/24</t>
+  </si>
+  <si>
+    <t>6.6/21</t>
+  </si>
+  <si>
+    <t>6.6/24</t>
+  </si>
+  <si>
+    <t>1/28</t>
+  </si>
+  <si>
+    <t>1/38</t>
+  </si>
+  <si>
+    <t>2/28</t>
+  </si>
+  <si>
+    <t>2/38</t>
+  </si>
+  <si>
+    <t>0/28</t>
+  </si>
+  <si>
+    <t>0/38</t>
+  </si>
+  <si>
+    <t>0.6/28</t>
+  </si>
+  <si>
+    <t>0.6/38</t>
+  </si>
+  <si>
+    <t>1/44</t>
+  </si>
+  <si>
+    <t>2/44</t>
+  </si>
+  <si>
+    <t>1/52</t>
+  </si>
+  <si>
+    <t>2/52</t>
+  </si>
+  <si>
+    <t>0/44</t>
+  </si>
+  <si>
+    <t>0/52</t>
   </si>
 </sst>
 </file>
@@ -866,9 +927,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -906,7 +967,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1012,7 +1073,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1154,7 +1215,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1894,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D0CA9D-08E8-E74D-9EAB-753CF0FAFD9E}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="139" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1938,16 +1999,28 @@
       </c>
       <c r="B2" s="1">
         <f>AVERAGE(C2:G2)</f>
-        <v>0</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="C2" s="1">
         <f>0/24</f>
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="D2" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1967,16 +2040,28 @@
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
-        <v>0</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="C3" s="1">
         <f>0/24</f>
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="D3" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1984,10 +2069,10 @@
         <v>81</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1996,16 +2081,28 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4" s="1">
         <f>0/24</f>
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="D4" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2013,10 +2110,10 @@
         <v>81</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2025,16 +2122,28 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.9999999999999996E-2</v>
       </c>
       <c r="C5" s="1">
         <f>0/24</f>
         <v>0</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="D5" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2042,10 +2151,10 @@
         <v>81</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2054,16 +2163,28 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
+        <v>9.1666666666666646E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:C12" si="1">2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="E6" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2071,10 +2192,10 @@
         <v>81</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2083,16 +2204,28 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
+        <v>9.1666666666666646E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="E7" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="F7" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2100,10 +2233,10 @@
         <v>81</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2112,16 +2245,28 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -2129,16 +2274,28 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="E9" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -2146,16 +2303,28 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="E10" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="F10" s="1">
+        <f>2/24</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -2163,16 +2332,28 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
+        <v>0.11666666666666665</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E11" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="F11" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -2180,16 +2361,28 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
+        <v>0.11666666666666665</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" ref="E12:E20" si="2">3/24</f>
+        <v>0.125</v>
+      </c>
+      <c r="F12" s="1">
         <f>2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -2197,16 +2390,28 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.15</v>
       </c>
       <c r="C13" s="1">
         <f>4/24</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="D13" s="1">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F13" s="1">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G13" s="1">
+        <f>3/24</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -2214,16 +2419,28 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="C14" s="1">
         <f>4/24</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="D14" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F14" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G14" s="1">
+        <f>4/24</f>
+        <v>0.16666666666666666</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2231,16 +2448,28 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.18333333333333335</v>
       </c>
       <c r="C15" s="1">
         <f>4/24</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="D15" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F15" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G15" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -2248,16 +2477,28 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="C16" s="1">
         <f>4/24</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="D16" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F16" s="1">
+        <f>6/24</f>
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="1">
+        <f>6/24</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -2265,16 +2506,28 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>0.2166666666666667</v>
       </c>
       <c r="C17" s="1">
         <f>5/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="D17" s="1">
+        <f>5/24</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F17" s="1">
+        <f>7/24</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" ref="G17:G21" si="3">6/24</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -2282,16 +2535,28 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>0.24166666666666664</v>
       </c>
       <c r="C18" s="1">
         <f>5/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="D18" s="1">
+        <f>7/24</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F18" s="1">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -2299,16 +2564,28 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>0.24166666666666664</v>
       </c>
       <c r="C19" s="1">
         <f>5/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="D19" s="1">
+        <f>7/24</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F19" s="1">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -2316,16 +2593,28 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>0.25</v>
       </c>
       <c r="C20" s="1">
         <f>5/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="D20" s="1">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="F20" s="1">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -2333,19 +2622,32 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="C21" s="1">
         <f>5/24</f>
         <v>0.20833333333333334</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="D21" s="1">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E21" s="1">
+        <f>6/24</f>
+        <v>0.25</v>
+      </c>
+      <c r="F21" s="1">
+        <f>8/24</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3076,7 +3378,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView zoomScale="154" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G21"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3117,15 +3419,30 @@
       <c r="A2">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="e">
+      <c r="B2" s="1">
         <f>AVERAGE(C2:G2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3133,25 +3450,40 @@
         <v>82</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
-      <c r="B3" s="1" t="e">
+      <c r="B3" s="1">
         <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:G21" si="1">0/38</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3159,25 +3491,40 @@
         <v>82</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>90</v>
       </c>
-      <c r="B4" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3185,25 +3532,40 @@
         <v>82</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>120</v>
       </c>
-      <c r="B5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>5.263157894736842E-3</v>
+      </c>
+      <c r="C5" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>0/38</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
@@ -3211,25 +3573,40 @@
         <v>82</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>150</v>
       </c>
-      <c r="B6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -3237,25 +3614,40 @@
         <v>82</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>180</v>
       </c>
-      <c r="B7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
@@ -3263,210 +3655,421 @@
         <v>82</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>210</v>
       </c>
-      <c r="B8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>240</v>
       </c>
-      <c r="B9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>270</v>
       </c>
-      <c r="B10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>300</v>
       </c>
-      <c r="B11" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>330</v>
       </c>
-      <c r="B12" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>360</v>
       </c>
-      <c r="B13" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>390</v>
       </c>
-      <c r="B14" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>420</v>
       </c>
-      <c r="B15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="C15" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>450</v>
       </c>
-      <c r="B16" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5789473684210527E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <f>2/38</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>480</v>
       </c>
-      <c r="B17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5789473684210527E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <f>2/38</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>510</v>
       </c>
-      <c r="B18" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5789473684210527E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <f>2/38</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>540</v>
       </c>
-      <c r="B19" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5789473684210527E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <f>2/38</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>570</v>
       </c>
-      <c r="B20" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5789473684210527E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <f>2/38</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>600</v>
       </c>
-      <c r="B21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5789473684210527E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <f>1/38</f>
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <f>2/38</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4197,7 +4800,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G21"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4238,15 +4841,30 @@
       <c r="A2">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="e">
+      <c r="B2" s="1">
         <f>AVERAGE(C2:G2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+        <v>3.8461538461538464E-3</v>
+      </c>
+      <c r="C2" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F21" si="0">1/52</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G2" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4254,25 +4872,40 @@
         <v>83</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
-      <c r="B3" s="1" t="e">
-        <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B21" si="1">AVERAGE(C3:G3)</f>
+        <v>3.8461538461538464E-3</v>
+      </c>
+      <c r="C3" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
@@ -4280,25 +4913,40 @@
         <v>83</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>90</v>
       </c>
-      <c r="B4" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="B4" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8461538461538464E-3</v>
+      </c>
+      <c r="C4" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4306,25 +4954,40 @@
         <v>83</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>120</v>
       </c>
-      <c r="B5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <f>1/52</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>1/52</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f>1/52</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
@@ -4332,25 +4995,40 @@
         <v>83</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>150</v>
       </c>
-      <c r="B6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:E21" si="2">1/52</f>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -4358,25 +5036,40 @@
         <v>83</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>180</v>
       </c>
-      <c r="B7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
@@ -4384,210 +5077,421 @@
         <v>83</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>210</v>
       </c>
-      <c r="B8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f>0/52</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>240</v>
       </c>
-      <c r="B9" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" ref="G9:G21" si="3">0/52</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>270</v>
       </c>
-      <c r="B10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>300</v>
       </c>
-      <c r="B11" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>330</v>
       </c>
-      <c r="B12" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>360</v>
       </c>
-      <c r="B13" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>390</v>
       </c>
-      <c r="B14" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>420</v>
       </c>
-      <c r="B15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>450</v>
       </c>
-      <c r="B16" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="B16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f>2/52</f>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>480</v>
       </c>
-      <c r="B17" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="B17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" ref="E17:E21" si="4">2/52</f>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>510</v>
       </c>
-      <c r="B18" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="B18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="4"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>540</v>
       </c>
-      <c r="B19" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="B19" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="4"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>570</v>
       </c>
-      <c r="B20" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="4"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>600</v>
       </c>
-      <c r="B21" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="4"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4596,7 +5500,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4806,12 +5710,203 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A06ECB-BB76-6147-8DB0-5BA023E66B2D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1">
+        <f>AVERAGE('VR Template-Random'!B2, 'XRI Assets-Random'!B2, 'EscapeProto-Random'!B2, 'EscapeRoom-Random'!B2, 'GameJam-Random'!B2, 'XRI Kit-Random'!B2, 'XRI Examples-Random'!B2)</f>
+        <v>3.3362652165975018E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <f>AVERAGE('VR Template-Random'!B3, 'XRI Assets-Random'!B3, 'EscapeProto-Random'!B3, 'EscapeRoom-Random'!B3, 'GameJam-Random'!B3, 'XRI Kit-Random'!B3, 'XRI Examples-Random'!B3)</f>
+        <v>4.2264940816804306E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>90</v>
+      </c>
+      <c r="B4" s="1">
+        <f>AVERAGE('VR Template-Random'!B4, 'XRI Assets-Random'!B4, 'EscapeProto-Random'!B4, 'EscapeRoom-Random'!B4, 'GameJam-Random'!B4, 'XRI Kit-Random'!B4, 'XRI Examples-Random'!B4)</f>
+        <v>6.2020858451033577E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1">
+        <f>AVERAGE('VR Template-Random'!B5, 'XRI Assets-Random'!B5, 'EscapeProto-Random'!B5, 'EscapeRoom-Random'!B5, 'GameJam-Random'!B5, 'XRI Kit-Random'!B5, 'XRI Examples-Random'!B5)</f>
+        <v>7.9143009100705333E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6" s="1">
+        <f>AVERAGE('VR Template-Random'!B6, 'XRI Assets-Random'!B6, 'EscapeProto-Random'!B6, 'EscapeRoom-Random'!B6, 'GameJam-Random'!B6, 'XRI Kit-Random'!B6, 'XRI Examples-Random'!B6)</f>
+        <v>9.3434350386114612E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7" s="1">
+        <f>AVERAGE('VR Template-Random'!B7, 'XRI Assets-Random'!B7, 'EscapeProto-Random'!B7, 'EscapeRoom-Random'!B7, 'GameJam-Random'!B7, 'XRI Kit-Random'!B7, 'XRI Examples-Random'!B7)</f>
+        <v>0.10690307120777663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE('VR Template-Random'!B8, 'XRI Assets-Random'!B8, 'EscapeProto-Random'!B8, 'EscapeRoom-Random'!B8, 'GameJam-Random'!B8, 'XRI Kit-Random'!B8, 'XRI Examples-Random'!B8)</f>
+        <v>0.10809354739825282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1">
+        <f>AVERAGE('VR Template-Random'!B9, 'XRI Assets-Random'!B9, 'EscapeProto-Random'!B9, 'EscapeRoom-Random'!B9, 'GameJam-Random'!B9, 'XRI Kit-Random'!B9, 'XRI Examples-Random'!B9)</f>
+        <v>0.11743204106543979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>270</v>
+      </c>
+      <c r="B10" s="1">
+        <f>AVERAGE('VR Template-Random'!B10, 'XRI Assets-Random'!B10, 'EscapeProto-Random'!B10, 'EscapeRoom-Random'!B10, 'GameJam-Random'!B10, 'XRI Kit-Random'!B10, 'XRI Examples-Random'!B10)</f>
+        <v>0.1292448577951851</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE('VR Template-Random'!B11, 'XRI Assets-Random'!B11, 'EscapeProto-Random'!B11, 'EscapeRoom-Random'!B11, 'GameJam-Random'!B11, 'XRI Kit-Random'!B11, 'XRI Examples-Random'!B11)</f>
+        <v>0.14953035112737803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>330</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE('VR Template-Random'!B12, 'XRI Assets-Random'!B12, 'EscapeProto-Random'!B12, 'EscapeRoom-Random'!B12, 'GameJam-Random'!B12, 'XRI Kit-Random'!B12, 'XRI Examples-Random'!B12)</f>
+        <v>0.15482183158724647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>360</v>
+      </c>
+      <c r="B13" s="1">
+        <f>AVERAGE('VR Template-Random'!B13, 'XRI Assets-Random'!B13, 'EscapeProto-Random'!B13, 'EscapeRoom-Random'!B13, 'GameJam-Random'!B13, 'XRI Kit-Random'!B13, 'XRI Examples-Random'!B13)</f>
+        <v>0.15958373634915124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>390</v>
+      </c>
+      <c r="B14" s="1">
+        <f>AVERAGE('VR Template-Random'!B14, 'XRI Assets-Random'!B14, 'EscapeProto-Random'!B14, 'EscapeRoom-Random'!B14, 'GameJam-Random'!B14, 'XRI Kit-Random'!B14, 'XRI Examples-Random'!B14)</f>
+        <v>0.1631551649205798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>420</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE('VR Template-Random'!B15, 'XRI Assets-Random'!B15, 'EscapeProto-Random'!B15, 'EscapeRoom-Random'!B15, 'GameJam-Random'!B15, 'XRI Kit-Random'!B15, 'XRI Examples-Random'!B15)</f>
+        <v>0.17088158882347429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>450</v>
+      </c>
+      <c r="B16" s="1">
+        <f>AVERAGE('VR Template-Random'!B16, 'XRI Assets-Random'!B16, 'EscapeProto-Random'!B16, 'EscapeRoom-Random'!B16, 'GameJam-Random'!B16, 'XRI Kit-Random'!B16, 'XRI Examples-Random'!B16)</f>
+        <v>0.17543628148584073</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>480</v>
+      </c>
+      <c r="B17" s="1">
+        <f>AVERAGE('VR Template-Random'!B17, 'XRI Assets-Random'!B17, 'EscapeProto-Random'!B17, 'EscapeRoom-Random'!B17, 'GameJam-Random'!B17, 'XRI Kit-Random'!B17, 'XRI Examples-Random'!B17)</f>
+        <v>0.1816147834209659</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>510</v>
+      </c>
+      <c r="B18" s="1">
+        <f>AVERAGE('VR Template-Random'!B18, 'XRI Assets-Random'!B18, 'EscapeProto-Random'!B18, 'EscapeRoom-Random'!B18, 'GameJam-Random'!B18, 'XRI Kit-Random'!B18, 'XRI Examples-Random'!B18)</f>
+        <v>0.18920186405474615</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>540</v>
+      </c>
+      <c r="B19" s="1">
+        <f>AVERAGE('VR Template-Random'!B19, 'XRI Assets-Random'!B19, 'EscapeProto-Random'!B19, 'EscapeRoom-Random'!B19, 'GameJam-Random'!B19, 'XRI Kit-Random'!B19, 'XRI Examples-Random'!B19)</f>
+        <v>0.19175494635636908</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>570</v>
+      </c>
+      <c r="B20" s="1">
+        <f>AVERAGE('VR Template-Random'!B20, 'XRI Assets-Random'!B20, 'EscapeProto-Random'!B20, 'EscapeRoom-Random'!B20, 'GameJam-Random'!B20, 'XRI Kit-Random'!B20, 'XRI Examples-Random'!B20)</f>
+        <v>0.19338162756320296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>600</v>
+      </c>
+      <c r="B21" s="1">
+        <f>AVERAGE('VR Template-Random'!B21, 'XRI Assets-Random'!B21, 'EscapeProto-Random'!B21, 'EscapeRoom-Random'!B21, 'GameJam-Random'!B21, 'XRI Kit-Random'!B21, 'XRI Examples-Random'!B21)</f>
+        <v>0.20100006934195011</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6264,7 +7359,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6379,7 +7474,7 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>56</v>
@@ -6414,14 +7509,14 @@
         <v>0.125</v>
       </c>
       <c r="G4" s="1">
-        <f>0/8</f>
+        <f t="shared" ref="G4:G9" si="2">0/8</f>
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>55</v>
@@ -6448,7 +7543,7 @@
         <v>0.125</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E21" si="2">2/8</f>
+        <f t="shared" ref="E5:E21" si="3">2/8</f>
         <v>0.25</v>
       </c>
       <c r="F5" s="1">
@@ -6456,14 +7551,14 @@
         <v>0.25</v>
       </c>
       <c r="G5" s="1">
-        <f>0/8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>56</v>
@@ -6490,7 +7585,7 @@
         <v>0.125</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="F6" s="1">
@@ -6498,14 +7593,14 @@
         <v>0.25</v>
       </c>
       <c r="G6" s="1">
-        <f>0/8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>56</v>
@@ -6524,7 +7619,7 @@
         <v>0.2</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:C21" si="3">2/8</f>
+        <f t="shared" ref="C7:C21" si="4">2/8</f>
         <v>0.25</v>
       </c>
       <c r="D7" s="1">
@@ -6532,7 +7627,7 @@
         <v>0.125</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="F7" s="1">
@@ -6540,14 +7635,14 @@
         <v>0.375</v>
       </c>
       <c r="G7" s="1">
-        <f>0/8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>57</v>
@@ -6566,23 +7661,23 @@
         <v>0.2</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
+        <f t="shared" ref="F8:G21" si="5">3/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" ref="F8:G21" si="4">3/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="G8" s="1">
-        <f>0/8</f>
         <v>0</v>
       </c>
     </row>
@@ -6595,23 +7690,23 @@
         <v>0.2</v>
       </c>
       <c r="C9" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
+        <f t="shared" si="5"/>
+        <v>0.375</v>
+      </c>
+      <c r="G9" s="1">
         <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="G9" s="1">
-        <f>0/8</f>
         <v>0</v>
       </c>
     </row>
@@ -6624,7 +7719,7 @@
         <v>0.25</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
       <c r="D10" s="1">
@@ -6632,11 +7727,11 @@
         <v>0.25</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="G10" s="1">
@@ -6653,7 +7748,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
       <c r="D11" s="1">
@@ -6661,11 +7756,11 @@
         <v>0.375</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
       <c r="G11" s="1">
@@ -6682,23 +7777,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C12" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" ref="D12:D21" si="6">3/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" ref="D12:D21" si="5">3/8</f>
+      <c r="F12" s="1">
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6711,23 +7806,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C13" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D13" s="1">
+      <c r="F13" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6740,23 +7835,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C14" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E14" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D14" s="1">
+      <c r="F14" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6769,23 +7864,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C15" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E15" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D15" s="1">
+      <c r="F15" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6798,23 +7893,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C16" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E16" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D16" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E16" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6827,23 +7922,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C17" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D17" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E17" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6856,23 +7951,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E18" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D18" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F18" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6885,23 +7980,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C19" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E19" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D19" s="1">
+      <c r="F19" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E19" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6914,23 +8009,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C20" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E20" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D20" s="1">
+      <c r="F20" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -6943,23 +8038,23 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C21" s="1">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.375</v>
+      </c>
+      <c r="E21" s="1">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="D21" s="1">
+      <c r="F21" s="1">
         <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
-      <c r="E21" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
       <c r="G21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.375</v>
       </c>
     </row>
@@ -7799,15 +8894,15 @@
         <v>4.7058823529411764E-2</v>
       </c>
       <c r="C2" s="1">
-        <f>1/17</f>
+        <f t="shared" ref="C2:E3" si="0">1/17</f>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="D2" s="1">
-        <f>1/17</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="E2" s="1">
-        <f>1/17</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="F2" s="1">
@@ -7836,19 +8931,19 @@
         <v>60</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
+        <f t="shared" ref="B3:B21" si="1">AVERAGE(C3:G3)</f>
         <v>5.8823529411764698E-2</v>
       </c>
       <c r="C3" s="1">
-        <f>1/17</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="D3" s="1">
-        <f>1/17</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="E3" s="1">
-        <f>1/17</f>
+        <f t="shared" si="0"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="F3" s="1">
@@ -7877,7 +8972,7 @@
         <v>90</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0588235294117646E-2</v>
       </c>
       <c r="C4" s="1">
@@ -7918,7 +9013,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0588235294117646E-2</v>
       </c>
       <c r="C5" s="1">
@@ -7959,7 +9054,7 @@
         <v>150</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.4117647058823528E-2</v>
       </c>
       <c r="C6" s="1">
@@ -8000,7 +9095,7 @@
         <v>180</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14117647058823529</v>
       </c>
       <c r="C7" s="1">
@@ -8041,7 +9136,7 @@
         <v>210</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14117647058823529</v>
       </c>
       <c r="C8" s="1">
@@ -8049,7 +9144,7 @@
         <v>0.11764705882352941</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:E21" si="1">3/17</f>
+        <f t="shared" ref="D8:E21" si="2">3/17</f>
         <v>0.17647058823529413</v>
       </c>
       <c r="E8" s="1">
@@ -8061,7 +9156,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G21" si="2">4/17</f>
+        <f t="shared" ref="G8:G21" si="3">4/17</f>
         <v>0.23529411764705882</v>
       </c>
       <c r="J8" s="2"/>
@@ -8073,7 +9168,7 @@
         <v>240</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15294117647058822</v>
       </c>
       <c r="C9" s="1">
@@ -8081,11 +9176,11 @@
         <v>0.11764705882352941</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="F9" s="1">
@@ -8093,7 +9188,7 @@
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J9" s="2"/>
@@ -8105,7 +9200,7 @@
         <v>270</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1764705882352941</v>
       </c>
       <c r="C10" s="1">
@@ -8113,7 +9208,7 @@
         <v>0.11764705882352941</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E10" s="1">
@@ -8121,11 +9216,11 @@
         <v>0.23529411764705882</v>
       </c>
       <c r="F10" s="1">
-        <f>2/17</f>
+        <f t="shared" ref="F10:F16" si="4">2/17</f>
         <v>0.11764705882352941</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J10" s="2"/>
@@ -8137,15 +9232,15 @@
         <v>300</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="C11" s="1">
-        <f>4/17</f>
+        <f t="shared" ref="C11:C16" si="5">4/17</f>
         <v>0.23529411764705882</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E11" s="1">
@@ -8153,11 +9248,11 @@
         <v>0.23529411764705882</v>
       </c>
       <c r="F11" s="1">
-        <f>2/17</f>
+        <f t="shared" si="4"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J11" s="2"/>
@@ -8169,15 +9264,15 @@
         <v>330</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.21176470588235294</v>
       </c>
       <c r="C12" s="1">
-        <f>4/17</f>
+        <f t="shared" si="5"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E12" s="1">
@@ -8185,11 +9280,11 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="F12" s="1">
-        <f>2/17</f>
+        <f t="shared" si="4"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J12" s="2"/>
@@ -8201,15 +9296,15 @@
         <v>360</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.21176470588235294</v>
       </c>
       <c r="C13" s="1">
-        <f>4/17</f>
+        <f t="shared" si="5"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E13" s="1">
@@ -8217,11 +9312,11 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="F13" s="1">
-        <f>2/17</f>
+        <f t="shared" si="4"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J13" s="2"/>
@@ -8233,15 +9328,15 @@
         <v>390</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.21176470588235294</v>
       </c>
       <c r="C14" s="1">
-        <f>4/17</f>
+        <f t="shared" si="5"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E14" s="1">
@@ -8249,11 +9344,11 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="F14" s="1">
-        <f>2/17</f>
+        <f t="shared" si="4"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J14" s="2"/>
@@ -8265,15 +9360,15 @@
         <v>420</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="C15" s="1">
-        <f>4/17</f>
+        <f t="shared" si="5"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E15" s="1">
@@ -8281,11 +9376,11 @@
         <v>0.41176470588235292</v>
       </c>
       <c r="F15" s="1">
-        <f>2/17</f>
+        <f t="shared" si="4"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J15" s="2"/>
@@ -8297,15 +9392,15 @@
         <v>450</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="C16" s="1">
-        <f>4/17</f>
+        <f t="shared" si="5"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E16" s="1">
@@ -8313,11 +9408,11 @@
         <v>0.41176470588235292</v>
       </c>
       <c r="F16" s="1">
-        <f>2/17</f>
+        <f t="shared" si="4"/>
         <v>0.11764705882352941</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J16" s="2"/>
@@ -8329,7 +9424,7 @@
         <v>480</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25882352941176473</v>
       </c>
       <c r="C17" s="1">
@@ -8337,7 +9432,7 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E17" s="1">
@@ -8349,7 +9444,7 @@
         <v>0.17647058823529413</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J17" s="2"/>
@@ -8361,7 +9456,7 @@
         <v>510</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.28235294117647058</v>
       </c>
       <c r="C18" s="1">
@@ -8369,7 +9464,7 @@
         <v>0.29411764705882354</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E18" s="1">
@@ -8381,7 +9476,7 @@
         <v>0.23529411764705882</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J18" s="2"/>
@@ -8393,7 +9488,7 @@
         <v>540</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29411764705882354</v>
       </c>
       <c r="C19" s="1">
@@ -8401,7 +9496,7 @@
         <v>0.35294117647058826</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E19" s="1">
@@ -8413,7 +9508,7 @@
         <v>0.23529411764705882</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J19" s="2"/>
@@ -8425,7 +9520,7 @@
         <v>570</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29411764705882354</v>
       </c>
       <c r="C20" s="1">
@@ -8433,7 +9528,7 @@
         <v>0.35294117647058826</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E20" s="1">
@@ -8445,7 +9540,7 @@
         <v>0.23529411764705882</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J20" s="2"/>
@@ -8457,7 +9552,7 @@
         <v>600</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.29411764705882354</v>
       </c>
       <c r="C21" s="1">
@@ -8465,7 +9560,7 @@
         <v>0.35294117647058826</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="E21" s="1">
@@ -8477,7 +9572,7 @@
         <v>0.23529411764705882</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="J21" s="2"/>
@@ -8495,7 +9590,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:L21"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9367,7 +10462,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="4">
-        <f>1/131</f>
+        <f t="shared" ref="G2:G9" si="0">1/131</f>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H2" s="3"/>
@@ -9389,7 +10484,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
+        <f t="shared" ref="B3:B21" si="1">AVERAGE(C3:G3)</f>
         <v>1.3740458015267177E-2</v>
       </c>
       <c r="C3" s="4">
@@ -9405,11 +10500,11 @@
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="F3" s="4">
-        <f>1/131</f>
+        <f t="shared" ref="F3:F8" si="2">1/131</f>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="G3" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H3" s="3"/>
@@ -9431,7 +10526,7 @@
         <v>90</v>
       </c>
       <c r="B4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5267175572519085E-2</v>
       </c>
       <c r="C4" s="4">
@@ -9447,11 +10542,11 @@
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="F4" s="4">
-        <f>1/131</f>
+        <f t="shared" si="2"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="G4" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H4" s="3"/>
@@ -9473,7 +10568,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8320610687022901E-2</v>
       </c>
       <c r="C5" s="4">
@@ -9485,15 +10580,15 @@
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="E5" s="4">
-        <f>3/131</f>
+        <f t="shared" ref="E5:E10" si="3">3/131</f>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="F5" s="4">
-        <f>1/131</f>
+        <f t="shared" si="2"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="G5" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H5" s="3"/>
@@ -9515,11 +10610,11 @@
         <v>150</v>
       </c>
       <c r="B6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="C6" s="4">
-        <f>4/131</f>
+        <f t="shared" ref="C6:C15" si="4">4/131</f>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D6" s="4">
@@ -9527,15 +10622,15 @@
         <v>4.5801526717557252E-2</v>
       </c>
       <c r="E6" s="4">
-        <f>3/131</f>
+        <f t="shared" si="3"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="F6" s="4">
-        <f>1/131</f>
+        <f t="shared" si="2"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="G6" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H6" s="3"/>
@@ -9557,11 +10652,11 @@
         <v>180</v>
       </c>
       <c r="B7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="C7" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D7" s="4">
@@ -9569,15 +10664,15 @@
         <v>4.5801526717557252E-2</v>
       </c>
       <c r="E7" s="4">
-        <f>3/131</f>
+        <f t="shared" si="3"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="F7" s="4">
-        <f>1/131</f>
+        <f t="shared" si="2"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="G7" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H7" s="3"/>
@@ -9599,11 +10694,11 @@
         <v>210</v>
       </c>
       <c r="B8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="C8" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D8" s="4">
@@ -9611,15 +10706,15 @@
         <v>4.5801526717557252E-2</v>
       </c>
       <c r="E8" s="4">
-        <f>3/131</f>
+        <f t="shared" si="3"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="F8" s="4">
-        <f>1/131</f>
+        <f t="shared" si="2"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="G8" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H8" s="3"/>
@@ -9633,11 +10728,11 @@
         <v>240</v>
       </c>
       <c r="B9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2061068702290078E-2</v>
       </c>
       <c r="C9" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D9" s="4">
@@ -9645,7 +10740,7 @@
         <v>6.8702290076335881E-2</v>
       </c>
       <c r="E9" s="4">
-        <f>3/131</f>
+        <f t="shared" si="3"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="F9" s="4">
@@ -9653,7 +10748,7 @@
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="G9" s="4">
-        <f>1/131</f>
+        <f t="shared" si="0"/>
         <v>7.6335877862595417E-3</v>
       </c>
       <c r="H9" s="3"/>
@@ -9667,11 +10762,11 @@
         <v>270</v>
       </c>
       <c r="B10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1221374045801527E-2</v>
       </c>
       <c r="C10" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D10" s="4">
@@ -9679,7 +10774,7 @@
         <v>9.9236641221374045E-2</v>
       </c>
       <c r="E10" s="4">
-        <f>3/131</f>
+        <f t="shared" si="3"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="F10" s="4">
@@ -9701,11 +10796,11 @@
         <v>300</v>
       </c>
       <c r="B11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5801526717557252E-2</v>
       </c>
       <c r="C11" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D11" s="4">
@@ -9735,11 +10830,11 @@
         <v>330</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8854961832061075E-2</v>
       </c>
       <c r="C12" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D12" s="4">
@@ -9751,11 +10846,11 @@
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="F12" s="4">
-        <f>5/131</f>
+        <f t="shared" ref="F12:F19" si="5">5/131</f>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" ref="G12:G21" si="1">3/131</f>
+        <f t="shared" ref="G12:G21" si="6">3/131</f>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H12" s="3"/>
@@ -9769,11 +10864,11 @@
         <v>360</v>
       </c>
       <c r="B13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8854961832061075E-2</v>
       </c>
       <c r="C13" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D13" s="4">
@@ -9785,11 +10880,11 @@
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="F13" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H13" s="3"/>
@@ -9803,11 +10898,11 @@
         <v>390</v>
       </c>
       <c r="B14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8854961832061075E-2</v>
       </c>
       <c r="C14" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D14" s="4">
@@ -9819,11 +10914,11 @@
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="F14" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H14" s="3"/>
@@ -9837,11 +10932,11 @@
         <v>420</v>
       </c>
       <c r="B15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8854961832061075E-2</v>
       </c>
       <c r="C15" s="4">
-        <f>4/131</f>
+        <f t="shared" si="4"/>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="D15" s="4">
@@ -9853,11 +10948,11 @@
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="F15" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H15" s="3"/>
@@ -9871,7 +10966,7 @@
         <v>450</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.4961832061068694E-2</v>
       </c>
       <c r="C16" s="4">
@@ -9887,11 +10982,11 @@
         <v>4.5801526717557252E-2</v>
       </c>
       <c r="F16" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H16" s="3"/>
@@ -9905,7 +11000,7 @@
         <v>480</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8015267175572517E-2</v>
       </c>
       <c r="C17" s="4">
@@ -9921,11 +11016,11 @@
         <v>6.1068702290076333E-2</v>
       </c>
       <c r="F17" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H17" s="3"/>
@@ -9939,7 +11034,7 @@
         <v>510</v>
       </c>
       <c r="B18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2595419847328235E-2</v>
       </c>
       <c r="C18" s="4">
@@ -9955,11 +11050,11 @@
         <v>6.8702290076335881E-2</v>
       </c>
       <c r="F18" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H18" s="3"/>
@@ -9973,7 +11068,7 @@
         <v>540</v>
       </c>
       <c r="B19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8702290076335881E-2</v>
       </c>
       <c r="C19" s="4">
@@ -9989,11 +11084,11 @@
         <v>6.8702290076335881E-2</v>
       </c>
       <c r="F19" s="4">
-        <f>5/131</f>
+        <f t="shared" si="5"/>
         <v>3.8167938931297711E-2</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H19" s="3"/>
@@ -10007,7 +11102,7 @@
         <v>570</v>
       </c>
       <c r="B20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.1755725190839698E-2</v>
       </c>
       <c r="C20" s="4">
@@ -10027,7 +11122,7 @@
         <v>5.3435114503816793E-2</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H20" s="3"/>
@@ -10041,7 +11136,7 @@
         <v>600</v>
       </c>
       <c r="B21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.786259541984733E-2</v>
       </c>
       <c r="C21" s="4">
@@ -10061,7 +11156,7 @@
         <v>6.1068702290076333E-2</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2.2900763358778626E-2</v>
       </c>
       <c r="H21" s="3"/>

</xml_diff>

<commit_message>
rename tool; update readme
</commit_message>
<xml_diff>
--- a/evaluation/results.xlsx
+++ b/evaluation/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruizhengu/Projects/InteractoBot/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B2AD0-2F34-5A48-BA90-252B0931E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F3D2BD-CA07-AC4F-81BA-0EDC1AC987BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="500" windowWidth="28800" windowHeight="26520" firstSheet="8" activeTab="15" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" activeTab="1" xr2:uid="{484EE131-55FD-F246-A82E-4E47E236206B}"/>
   </bookViews>
   <sheets>
     <sheet name="VR Template-InteractoBot" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="111">
   <si>
     <t>Time</t>
   </si>
@@ -185,31 +185,7 @@
     <t>3/8</t>
   </si>
   <si>
-    <t>4/8</t>
-  </si>
-  <si>
-    <t>4/9</t>
-  </si>
-  <si>
-    <t>5/8</t>
-  </si>
-  <si>
-    <t>5/9</t>
-  </si>
-  <si>
-    <t>3/9</t>
-  </si>
-  <si>
     <t>2/8</t>
-  </si>
-  <si>
-    <t>2/9</t>
-  </si>
-  <si>
-    <t>3.6/8</t>
-  </si>
-  <si>
-    <t>3.6/9</t>
   </si>
   <si>
     <t>0/2</t>
@@ -366,6 +342,45 @@
   </si>
   <si>
     <t>0/52</t>
+  </si>
+  <si>
+    <t>Run 6</t>
+  </si>
+  <si>
+    <t>Run 7</t>
+  </si>
+  <si>
+    <t>Run 8</t>
+  </si>
+  <si>
+    <t>Run 9</t>
+  </si>
+  <si>
+    <t>Run 10</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>4.2/8</t>
+  </si>
+  <si>
+    <t>4.2/9</t>
+  </si>
+  <si>
+    <t>Tempt 6</t>
+  </si>
+  <si>
+    <t>Tempt 7</t>
+  </si>
+  <si>
+    <t>Tempt 8</t>
+  </si>
+  <si>
+    <t>Tempt 9</t>
+  </si>
+  <si>
+    <t>Tempt 10</t>
   </si>
 </sst>
 </file>
@@ -855,7 +870,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -868,6 +883,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2006,32 +2030,32 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <f>1/24</f>
+        <f t="shared" ref="D2:G3" si="0">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E2" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G2" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2039,7 +2063,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B21" si="0">AVERAGE(C3:G3)</f>
+        <f t="shared" ref="B3:B21" si="1">AVERAGE(C3:G3)</f>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="C3" s="1">
@@ -2047,32 +2071,32 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E3" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G3" s="1">
-        <f>1/24</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -2080,7 +2104,7 @@
         <v>90</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C4" s="1">
@@ -2092,7 +2116,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E4" s="1">
-        <f>2/24</f>
+        <f t="shared" ref="E4:E10" si="2">2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F4" s="1">
@@ -2107,13 +2131,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2121,7 +2145,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="C5" s="1">
@@ -2133,7 +2157,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E5" s="1">
-        <f>2/24</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F5" s="1">
@@ -2148,13 +2172,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2162,11 +2186,11 @@
         <v>150</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1666666666666646E-2</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C12" si="1">2/24</f>
+        <f t="shared" ref="C6:C12" si="3">2/24</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D6" s="1">
@@ -2174,7 +2198,7 @@
         <v>0.125</v>
       </c>
       <c r="E6" s="1">
-        <f>2/24</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F6" s="1">
@@ -2189,13 +2213,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2203,11 +2227,11 @@
         <v>180</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.1666666666666646E-2</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D7" s="1">
@@ -2215,7 +2239,7 @@
         <v>0.125</v>
       </c>
       <c r="E7" s="1">
-        <f>2/24</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F7" s="1">
@@ -2230,13 +2254,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2244,11 +2268,11 @@
         <v>210</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D8" s="1">
@@ -2256,7 +2280,7 @@
         <v>0.125</v>
       </c>
       <c r="E8" s="1">
-        <f>2/24</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F8" s="1">
@@ -2264,7 +2288,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G8" s="1">
-        <f>3/24</f>
+        <f t="shared" ref="G8:G13" si="4">3/24</f>
         <v>0.125</v>
       </c>
     </row>
@@ -2273,11 +2297,11 @@
         <v>240</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D9" s="1">
@@ -2285,7 +2309,7 @@
         <v>0.125</v>
       </c>
       <c r="E9" s="1">
-        <f>2/24</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F9" s="1">
@@ -2293,7 +2317,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G9" s="1">
-        <f>3/24</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
     </row>
@@ -2302,11 +2326,11 @@
         <v>270</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D10" s="1">
@@ -2314,7 +2338,7 @@
         <v>0.125</v>
       </c>
       <c r="E10" s="1">
-        <f>2/24</f>
+        <f t="shared" si="2"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F10" s="1">
@@ -2322,7 +2346,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G10" s="1">
-        <f>3/24</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
     </row>
@@ -2331,11 +2355,11 @@
         <v>300</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11666666666666665</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D11" s="1">
@@ -2351,7 +2375,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G11" s="1">
-        <f>3/24</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
     </row>
@@ -2360,11 +2384,11 @@
         <v>330</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11666666666666665</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D12" s="1">
@@ -2372,7 +2396,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" ref="E12:E20" si="2">3/24</f>
+        <f t="shared" ref="E12:E20" si="5">3/24</f>
         <v>0.125</v>
       </c>
       <c r="F12" s="1">
@@ -2380,7 +2404,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G12" s="1">
-        <f>3/24</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
     </row>
@@ -2389,7 +2413,7 @@
         <v>360</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
       <c r="C13" s="1">
@@ -2401,7 +2425,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F13" s="1">
@@ -2409,7 +2433,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="G13" s="1">
-        <f>3/24</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
     </row>
@@ -2418,7 +2442,7 @@
         <v>390</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.17499999999999999</v>
       </c>
       <c r="C14" s="1">
@@ -2430,7 +2454,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F14" s="1">
@@ -2447,7 +2471,7 @@
         <v>420</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.18333333333333335</v>
       </c>
       <c r="C15" s="1">
@@ -2459,7 +2483,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F15" s="1">
@@ -2476,7 +2500,7 @@
         <v>450</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="C16" s="1">
@@ -2488,7 +2512,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F16" s="1">
@@ -2505,7 +2529,7 @@
         <v>480</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2166666666666667</v>
       </c>
       <c r="C17" s="1">
@@ -2517,7 +2541,7 @@
         <v>0.20833333333333334</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F17" s="1">
@@ -2525,7 +2549,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17:G21" si="3">6/24</f>
+        <f t="shared" ref="G17:G21" si="6">6/24</f>
         <v>0.25</v>
       </c>
     </row>
@@ -2534,7 +2558,7 @@
         <v>510</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24166666666666664</v>
       </c>
       <c r="C18" s="1">
@@ -2546,7 +2570,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F18" s="1">
@@ -2554,7 +2578,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
     </row>
@@ -2563,7 +2587,7 @@
         <v>540</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.24166666666666664</v>
       </c>
       <c r="C19" s="1">
@@ -2575,7 +2599,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F19" s="1">
@@ -2583,7 +2607,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
     </row>
@@ -2592,7 +2616,7 @@
         <v>570</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="C20" s="1">
@@ -2604,7 +2628,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
       <c r="F20" s="1">
@@ -2612,7 +2636,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
     </row>
@@ -2621,7 +2645,7 @@
         <v>600</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="C21" s="1">
@@ -2641,7 +2665,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.25</v>
       </c>
     </row>
@@ -3447,13 +3471,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -3488,13 +3512,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -3529,13 +3553,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -3547,7 +3571,7 @@
         <v>5.263157894736842E-3</v>
       </c>
       <c r="C5" s="1">
-        <f>1/38</f>
+        <f t="shared" ref="C5:C21" si="2">1/38</f>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D5" s="1">
@@ -3570,13 +3594,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -3588,11 +3612,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C6" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D6" s="1">
-        <f>1/38</f>
+        <f t="shared" ref="D6:D15" si="3">1/38</f>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E6" s="1">
@@ -3611,13 +3635,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -3629,11 +3653,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C7" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D7" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E7" s="1">
@@ -3652,13 +3676,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3670,11 +3694,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C8" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D8" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E8" s="1">
@@ -3699,11 +3723,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C9" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D9" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E9" s="1">
@@ -3728,11 +3752,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C10" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D10" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E10" s="1">
@@ -3757,11 +3781,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C11" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D11" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E11" s="1">
@@ -3786,11 +3810,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C12" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D12" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E12" s="1">
@@ -3815,11 +3839,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C13" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D13" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E13" s="1">
@@ -3844,11 +3868,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C14" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D14" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E14" s="1">
@@ -3873,11 +3897,11 @@
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="C15" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D15" s="1">
-        <f>1/38</f>
+        <f t="shared" si="3"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="E15" s="1">
@@ -3902,11 +3926,11 @@
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="C16" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D16" s="1">
-        <f>2/38</f>
+        <f t="shared" ref="D16:D21" si="4">2/38</f>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E16" s="1">
@@ -3931,11 +3955,11 @@
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="C17" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D17" s="1">
-        <f>2/38</f>
+        <f t="shared" si="4"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E17" s="1">
@@ -3960,11 +3984,11 @@
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="C18" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D18" s="1">
-        <f>2/38</f>
+        <f t="shared" si="4"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E18" s="1">
@@ -3989,11 +4013,11 @@
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="C19" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D19" s="1">
-        <f>2/38</f>
+        <f t="shared" si="4"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E19" s="1">
@@ -4018,11 +4042,11 @@
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="C20" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D20" s="1">
-        <f>2/38</f>
+        <f t="shared" si="4"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E20" s="1">
@@ -4047,11 +4071,11 @@
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="C21" s="1">
-        <f>1/38</f>
+        <f t="shared" si="2"/>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="D21" s="1">
-        <f>2/38</f>
+        <f t="shared" si="4"/>
         <v>5.2631578947368418E-2</v>
       </c>
       <c r="E21" s="1">
@@ -4846,36 +4870,36 @@
         <v>3.8461538461538464E-3</v>
       </c>
       <c r="C2" s="1">
-        <f>0/52</f>
+        <f t="shared" ref="C2:E4" si="0">0/52</f>
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F21" si="0">1/52</f>
+        <f t="shared" ref="F2:F21" si="1">1/52</f>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G2" s="1">
-        <f>0/52</f>
+        <f t="shared" ref="G2:G8" si="2">0/52</f>
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -4883,40 +4907,40 @@
         <v>60</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B21" si="1">AVERAGE(C3:G3)</f>
+        <f t="shared" ref="B3:B21" si="3">AVERAGE(C3:G3)</f>
         <v>3.8461538461538464E-3</v>
       </c>
       <c r="C3" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G3" s="1">
-        <f>0/52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -4924,40 +4948,40 @@
         <v>90</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.8461538461538464E-3</v>
       </c>
       <c r="C4" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f>0/52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G4" s="1">
-        <f>0/52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -4965,7 +4989,7 @@
         <v>120</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C5" s="1">
@@ -4981,24 +5005,24 @@
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G5" s="1">
-        <f>0/52</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -5006,40 +5030,40 @@
         <v>150</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:E21" si="2">1/52</f>
+        <f t="shared" ref="C6:E21" si="4">1/52</f>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G6" s="1">
         <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="G6" s="1">
-        <f>0/52</f>
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -5047,40 +5071,40 @@
         <v>180</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C7" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G7" s="1">
         <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="G7" s="1">
-        <f>0/52</f>
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -5088,27 +5112,27 @@
         <v>210</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="4"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9230769230769232E-2</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>1.9230769230769232E-2</v>
-      </c>
-      <c r="G8" s="1">
-        <f>0/52</f>
         <v>0</v>
       </c>
     </row>
@@ -5117,27 +5141,27 @@
         <v>240</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9:G21" si="3">0/52</f>
+        <f t="shared" ref="G9:G21" si="5">0/52</f>
         <v>0</v>
       </c>
     </row>
@@ -5146,27 +5170,27 @@
         <v>270</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5175,27 +5199,27 @@
         <v>300</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5204,27 +5228,27 @@
         <v>330</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5233,27 +5257,27 @@
         <v>360</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5262,27 +5286,27 @@
         <v>390</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5291,27 +5315,27 @@
         <v>420</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5320,15 +5344,15 @@
         <v>450</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E16" s="1">
@@ -5336,11 +5360,11 @@
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5349,27 +5373,27 @@
         <v>480</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ref="E17:E21" si="4">2/52</f>
+        <f t="shared" ref="E17:E21" si="6">2/52</f>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5378,27 +5402,27 @@
         <v>510</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5407,27 +5431,27 @@
         <v>540</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5436,27 +5460,27 @@
         <v>570</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5465,27 +5489,27 @@
         <v>600</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3.8461538461538464E-2</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9230769230769232E-2</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -5712,7 +5736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A06ECB-BB76-6147-8DB0-5BA023E66B2D}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -5913,19 +5937,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C56133-D0E1-9841-A980-CD948866944A}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="7" width="10.83203125" style="1"/>
-    <col min="9" max="12" width="10.83203125" style="2"/>
+    <col min="2" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="17" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5947,19 +5971,33 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>30</v>
       </c>
@@ -5987,22 +6025,40 @@
         <f>2/9</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="I2" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K2" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="L2" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="9">
+        <v>1</v>
+      </c>
+      <c r="P2" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
@@ -6030,22 +6086,40 @@
         <f t="shared" ref="G3:G21" si="3">3/9</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I3" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K3" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L3" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="9">
+        <v>0</v>
+      </c>
+      <c r="P3" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>90</v>
       </c>
@@ -6073,22 +6147,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I4" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K4" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L4" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
         <v>4</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q4" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>120</v>
       </c>
@@ -6116,22 +6208,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I5" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K5" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L5" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="9">
+        <v>0</v>
+      </c>
+      <c r="P5" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>150</v>
       </c>
@@ -6159,22 +6269,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I6" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K6" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L6" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0</v>
+      </c>
+      <c r="P6" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>180</v>
       </c>
@@ -6202,22 +6330,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I7" s="1">
+        <f>0/9</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K7" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="L7" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="9">
+        <v>0</v>
+      </c>
+      <c r="P7" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>210</v>
       </c>
@@ -6245,8 +6391,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="I8" s="1">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J8" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K8" s="1">
+        <f>6/9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L8" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>240</v>
       </c>
@@ -6274,8 +6452,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <f>5/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I9" s="1">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J9" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" ref="J9:K21" si="7">6/9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L9" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="O9" s="10">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>270</v>
       </c>
@@ -6303,8 +6513,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <f t="shared" ref="H10:J21" si="8">5/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I10" s="1">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J10" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10:L21" si="9">4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>300</v>
       </c>
@@ -6332,8 +6574,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I11" s="1">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J11" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="O11" s="10">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>330</v>
       </c>
@@ -6361,8 +6635,40 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H12" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I12" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J12" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="O12" s="10">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>360</v>
       </c>
@@ -6390,8 +6696,43 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H13" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I13" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J13" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="9">
+        <f>AVERAGE(O3:O12)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="9">
+        <f>AVERAGE(P3:P12)</f>
+        <v>4.2</v>
+      </c>
+      <c r="Q13" s="9">
+        <f>AVERAGE(Q3:Q12)</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>390</v>
       </c>
@@ -6419,8 +6760,37 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I14" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J14" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>420</v>
       </c>
@@ -6448,8 +6818,28 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H15" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I15" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J15" s="1">
+        <f>4/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>450</v>
       </c>
@@ -6477,8 +6867,28 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I16" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>480</v>
       </c>
@@ -6506,8 +6916,28 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I17" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>510</v>
       </c>
@@ -6535,8 +6965,28 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I18" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>540</v>
       </c>
@@ -6564,8 +7014,28 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I19" s="1">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>570</v>
       </c>
@@ -6593,8 +7063,28 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I20" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>600</v>
       </c>
@@ -6622,8 +7112,29 @@
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
+      <c r="H21" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I21" s="1">
+        <f>3/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="9"/>
+        <v>0.44444444444444442</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -7432,13 +7943,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M2" s="1"/>
     </row>
@@ -7474,10 +7985,10 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>44</v>
@@ -7516,13 +8027,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="M4" s="1"/>
     </row>
@@ -7558,10 +8069,10 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>44</v>
@@ -7600,10 +8111,10 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>44</v>
@@ -7642,13 +8153,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="M7" s="1"/>
     </row>
@@ -8917,13 +9428,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -8958,13 +9469,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -8999,13 +9510,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -9040,13 +9551,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -9081,13 +9592,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -9122,13 +9633,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -10470,13 +10981,13 @@
         <v>2</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -10512,13 +11023,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -10554,13 +11065,13 @@
         <v>4</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -10596,13 +11107,13 @@
         <v>5</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -10638,13 +11149,13 @@
         <v>6</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -10680,13 +11191,13 @@
         <v>13</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>